<commit_message>
Add Chart Axis Option textRotation
Fix #2705. Add to Axis class, Reader Xlsx Chart, and Writer Xlsx Chart. Add feature to an existing 32* sample, to an existing 33* sample, and a formal unit test.
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteScatterChart8.xlsx
+++ b/samples/templates/32readwriteScatterChart8.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0039B254-08BC-4CF2-A3C0-399F49B2E673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D83E5-932A-4719-B99E-3F107EA35C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -75,7 +75,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,6 +419,16 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="75089408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -825,7 +835,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add Chart Axis Option textRotation (#2940)
Fix #2705. Add to Axis class, Reader Xlsx Chart, and Writer Xlsx Chart. Add feature to an existing 32* sample, to an existing 33* sample, and a formal unit test.
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteScatterChart8.xlsx
+++ b/samples/templates/32readwriteScatterChart8.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0039B254-08BC-4CF2-A3C0-399F49B2E673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D83E5-932A-4719-B99E-3F107EA35C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -75,7 +75,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,6 +419,16 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="75089408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -825,7 +835,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>